<commit_message>
Bug fixed and Bot basic finished.
</commit_message>
<xml_diff>
--- a/影都第二次公会战数据.xlsx
+++ b/影都第二次公会战数据.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Personal\University\Code\PY\PCR_Bot\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9343FF04-B198-4778-8A45-ACB6F7CE7CB3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDA1DE29-DDB3-446D-A678-71AFB74E16A0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="22695" windowHeight="15196" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="22695" windowHeight="15196" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Boss" sheetId="2" r:id="rId1"/>
-    <sheet name="Template" sheetId="1" r:id="rId2"/>
+    <sheet name="Boss" sheetId="1" r:id="rId1"/>
+    <sheet name="Template" sheetId="2" r:id="rId2"/>
+    <sheet name="RockyQº" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -29,7 +30,22 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="22">
+  <si>
+    <t>飞龙</t>
+  </si>
+  <si>
+    <t>狂暴格里芬</t>
+  </si>
+  <si>
+    <t>兽人酋长</t>
+  </si>
+  <si>
+    <t>圣灵角鹿</t>
+  </si>
+  <si>
+    <t>牛头怪</t>
+  </si>
   <si>
     <t xml:space="preserve">       日期
 刀序</t>
@@ -80,24 +96,7 @@
     <t>涨幅</t>
   </si>
   <si>
-    <t>飞龙</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>狂暴格里芬</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>兽人酋长</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>圣灵角鹿</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>牛头怪</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <t>RockyQº</t>
   </si>
 </sst>
 </file>
@@ -353,7 +352,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-7340-4F16-A8D5-02F70AD6C8E6}"/>
+              <c16:uniqueId val="{00000000-887F-4097-B9AC-598CC1B7C9C3}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -424,7 +423,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-7340-4F16-A8D5-02F70AD6C8E6}"/>
+              <c16:uniqueId val="{00000001-887F-4097-B9AC-598CC1B7C9C3}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -495,7 +494,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000002-7340-4F16-A8D5-02F70AD6C8E6}"/>
+              <c16:uniqueId val="{00000002-887F-4097-B9AC-598CC1B7C9C3}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -537,7 +536,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000003-7340-4F16-A8D5-02F70AD6C8E6}"/>
+              <c16:uniqueId val="{00000003-887F-4097-B9AC-598CC1B7C9C3}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -724,7 +723,7 @@
         <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1041,21 +1040,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FC3CF3A3-681F-48BC-A676-4627A984E22F}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.9" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="10.796875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.796875" style="7" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="B1">
         <v>6000000</v>
@@ -1063,7 +1062,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
-        <v>17</v>
+        <v>1</v>
       </c>
       <c r="B2">
         <v>8000000</v>
@@ -1071,7 +1070,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
-        <v>18</v>
+        <v>2</v>
       </c>
       <c r="B3">
         <v>10000000</v>
@@ -1079,7 +1078,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
-        <v>19</v>
+        <v>3</v>
       </c>
       <c r="B4">
         <v>12000000</v>
@@ -1087,7 +1086,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A5" t="s">
-        <v>20</v>
+        <v>4</v>
       </c>
       <c r="B5">
         <v>20000000</v>
@@ -1096,16 +1095,16 @@
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="B1:L21"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L12" sqref="L12"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="M13" sqref="M13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.9" x14ac:dyDescent="0.4"/>
@@ -1121,33 +1120,33 @@
     </row>
     <row r="3" spans="2:12" ht="33" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B3" s="3" t="s">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="E3" s="6" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="F3" s="6" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="G3" s="6" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="H3" s="6" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="I3" s="6" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
     </row>
     <row r="4" spans="2:12" ht="26" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B4" s="5" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="C4" s="6"/>
       <c r="D4" s="6"/>
@@ -1159,7 +1158,7 @@
     </row>
     <row r="5" spans="2:12" ht="26" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B5" s="6" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="C5" s="6"/>
       <c r="D5" s="6"/>
@@ -1169,7 +1168,7 @@
       <c r="H5" s="6"/>
       <c r="I5" s="6"/>
       <c r="K5" s="4" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="L5" s="4">
         <v>0</v>
@@ -1177,7 +1176,7 @@
     </row>
     <row r="6" spans="2:12" ht="26" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B6" s="5" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="C6" s="6"/>
       <c r="D6" s="6"/>
@@ -1187,7 +1186,7 @@
       <c r="H6" s="6"/>
       <c r="I6" s="6"/>
       <c r="K6" s="4" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="L6" s="4">
         <v>0</v>
@@ -1195,7 +1194,7 @@
     </row>
     <row r="7" spans="2:12" ht="26" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B7" s="6" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="C7" s="6"/>
       <c r="D7" s="6"/>
@@ -1207,7 +1206,7 @@
     </row>
     <row r="8" spans="2:12" ht="26" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B8" s="5" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="C8" s="6"/>
       <c r="D8" s="6"/>
@@ -1219,7 +1218,7 @@
     </row>
     <row r="9" spans="2:12" ht="26" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B9" s="6" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="C9" s="6"/>
       <c r="D9" s="6"/>
@@ -1231,7 +1230,7 @@
     </row>
     <row r="10" spans="2:12" ht="26" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B10" s="6" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="C10" s="6">
         <f t="shared" ref="C10:I10" si="0">SUM(C5,C7,C9)</f>
@@ -1264,7 +1263,7 @@
     </row>
     <row r="11" spans="2:12" ht="26" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B11" s="6" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="C11" s="6"/>
       <c r="D11" s="6" t="e">
@@ -1308,4 +1307,215 @@
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="B1:L21"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F17" sqref="F17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.9" x14ac:dyDescent="0.4"/>
+  <cols>
+    <col min="3" max="9" width="13.06640625" style="7" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:12" ht="44.65" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B1" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="2:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B2" s="1"/>
+    </row>
+    <row r="3" spans="2:12" ht="33" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B3" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="E3" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="F3" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="G3" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="H3" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="I3" s="6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="2:12" ht="26" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B4" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" s="6"/>
+      <c r="D4" s="6"/>
+      <c r="E4" s="6"/>
+      <c r="F4" s="6"/>
+      <c r="G4" s="6"/>
+      <c r="H4" s="6"/>
+      <c r="I4" s="6"/>
+    </row>
+    <row r="5" spans="2:12" ht="26" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B5" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" s="6"/>
+      <c r="D5" s="6"/>
+      <c r="E5" s="6"/>
+      <c r="F5" s="6"/>
+      <c r="G5" s="6"/>
+      <c r="H5" s="6"/>
+      <c r="I5" s="6"/>
+      <c r="K5" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="L5" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="2:12" ht="26" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B6" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" s="6"/>
+      <c r="D6" s="6"/>
+      <c r="E6" s="6"/>
+      <c r="F6" s="6"/>
+      <c r="G6" s="6"/>
+      <c r="H6" s="6"/>
+      <c r="I6" s="6"/>
+      <c r="K6" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="L6" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="2:12" ht="26" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B7" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="C7" s="6"/>
+      <c r="D7" s="6"/>
+      <c r="E7" s="6"/>
+      <c r="F7" s="6"/>
+      <c r="G7" s="6"/>
+      <c r="H7" s="6"/>
+      <c r="I7" s="6"/>
+    </row>
+    <row r="8" spans="2:12" ht="26" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B8" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C8" s="6"/>
+      <c r="D8" s="6"/>
+      <c r="E8" s="6"/>
+      <c r="F8" s="6"/>
+      <c r="G8" s="6"/>
+      <c r="H8" s="6"/>
+      <c r="I8" s="6"/>
+    </row>
+    <row r="9" spans="2:12" ht="26" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B9" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="C9" s="6"/>
+      <c r="D9" s="6"/>
+      <c r="E9" s="6"/>
+      <c r="F9" s="6"/>
+      <c r="G9" s="6"/>
+      <c r="H9" s="6"/>
+      <c r="I9" s="6"/>
+    </row>
+    <row r="10" spans="2:12" ht="26" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B10" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="C10" s="6">
+        <f t="shared" ref="C10:I10" si="0">SUM(C5,C7,C9)</f>
+        <v>0</v>
+      </c>
+      <c r="D10" s="6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E10" s="6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F10" s="6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G10" s="6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H10" s="6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I10" s="6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="2:12" ht="26" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B11" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="C11" s="6"/>
+      <c r="D11" s="6" t="e">
+        <f t="shared" ref="D11:I11" si="1">(D10-C10)/C10</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="E11" s="6" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="F11" s="6" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G11" s="6" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H11" s="6" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I11" s="6" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="12" spans="2:12" ht="25.05" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="13" spans="2:12" ht="25.05" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="14" spans="2:12" ht="25.05" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="15" spans="2:12" ht="25.05" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="16" spans="2:12" ht="25.05" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="17" ht="25.05" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="18" ht="25.05" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="19" ht="25.05" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="20" ht="25.05" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="21" ht="20" customHeight="1" x14ac:dyDescent="0.4"/>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait"/>
+</worksheet>
 </file>
</xml_diff>